<commit_message>
update all the stimuli options
</commit_message>
<xml_diff>
--- a/03_Materials/stimuli_options.xlsx
+++ b/03_Materials/stimuli_options.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/GitHub/SPAML/SPAML-PSA/stimuli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/GitHub/SPAML/SPAML-PSA/03_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26899C86-AD3C-B642-804B-F0FDEF2B1698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A874944F-8FAD-6849-9689-3FC317312FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="21600" windowHeight="38400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="udpipe_languages" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">udpipe_languages!$A$1:$L$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">udpipe_languages!$A$2:$Q$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="514">
   <si>
     <t>language</t>
   </si>
@@ -1560,7 +1560,22 @@
     <t>https://hdl.handle.net/1839/6482e475-7d1f-4e2a-8de7-5affd860b402@download</t>
   </si>
   <si>
-    <t>less_50K</t>
+    <t>Usable</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>subs_vec_download</t>
+  </si>
+  <si>
+    <t>subs_count_download</t>
+  </si>
+  <si>
+    <t>wiki_vec_download</t>
+  </si>
+  <si>
+    <t>wiki_count_download</t>
   </si>
 </sst>
 </file>
@@ -2103,7 +2118,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2424,23 +2449,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="28.5" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.5" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>282</v>
       </c>
@@ -2477,8 +2507,23 @@
       <c r="L1" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>509</v>
+      </c>
+      <c r="N1" t="s">
+        <v>511</v>
+      </c>
+      <c r="O1" t="s">
+        <v>513</v>
+      </c>
+      <c r="P1" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2512,8 +2557,26 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2547,8 +2610,26 @@
       <c r="K3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2582,8 +2663,26 @@
       <c r="K4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2617,8 +2716,14 @@
       <c r="K5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2652,8 +2757,14 @@
       <c r="K6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2687,8 +2798,14 @@
       <c r="K7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2722,8 +2839,26 @@
       <c r="K8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2757,8 +2892,26 @@
       <c r="K9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2792,8 +2945,26 @@
       <c r="K10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2827,8 +2998,26 @@
       <c r="K11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2862,8 +3051,26 @@
       <c r="K12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2897,8 +3104,26 @@
       <c r="K13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2932,8 +3157,14 @@
       <c r="K14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2967,8 +3198,26 @@
       <c r="K15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -3002,8 +3251,26 @@
       <c r="K16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -3037,8 +3304,26 @@
       <c r="K17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -3072,8 +3357,26 @@
       <c r="K18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -3107,8 +3410,26 @@
       <c r="K19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O19" t="s">
+        <v>24</v>
+      </c>
+      <c r="P19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -3142,8 +3463,26 @@
       <c r="K20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -3177,8 +3516,26 @@
       <c r="K21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -3212,8 +3569,26 @@
       <c r="K22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O22" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -3247,8 +3622,26 @@
       <c r="K23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -3282,8 +3675,26 @@
       <c r="K24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -3317,8 +3728,26 @@
       <c r="K25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" t="s">
+        <v>9</v>
+      </c>
+      <c r="O25" t="s">
+        <v>24</v>
+      </c>
+      <c r="P25" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -3352,8 +3781,26 @@
       <c r="K26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -3387,8 +3834,26 @@
       <c r="K27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" t="s">
+        <v>9</v>
+      </c>
+      <c r="O27" t="s">
+        <v>24</v>
+      </c>
+      <c r="P27" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -3422,8 +3887,14 @@
       <c r="K28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3457,8 +3928,26 @@
       <c r="K29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" t="s">
+        <v>9</v>
+      </c>
+      <c r="N29" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -3480,8 +3969,26 @@
       <c r="K30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" t="s">
+        <v>24</v>
+      </c>
+      <c r="P30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3515,8 +4022,14 @@
       <c r="K31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -3550,8 +4063,14 @@
       <c r="K32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -3585,8 +4104,26 @@
       <c r="K33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" t="s">
+        <v>24</v>
+      </c>
+      <c r="P33" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -3620,8 +4157,26 @@
       <c r="K34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" t="s">
+        <v>9</v>
+      </c>
+      <c r="N34" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -3655,8 +4210,26 @@
       <c r="K35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" t="s">
+        <v>9</v>
+      </c>
+      <c r="O35" t="s">
+        <v>24</v>
+      </c>
+      <c r="P35" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -3690,8 +4263,14 @@
       <c r="K36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>167</v>
       </c>
@@ -3725,8 +4304,14 @@
       <c r="K37" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>171</v>
       </c>
@@ -3760,8 +4345,14 @@
       <c r="K38" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -3795,8 +4386,26 @@
       <c r="K39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" t="s">
+        <v>9</v>
+      </c>
+      <c r="N39" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -3830,8 +4439,26 @@
       <c r="K40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" t="s">
+        <v>9</v>
+      </c>
+      <c r="O40" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -3865,8 +4492,26 @@
       <c r="K41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" t="s">
+        <v>9</v>
+      </c>
+      <c r="O41" t="s">
+        <v>24</v>
+      </c>
+      <c r="P41" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>188</v>
       </c>
@@ -3900,8 +4545,26 @@
       <c r="K42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" t="s">
+        <v>9</v>
+      </c>
+      <c r="O42" t="s">
+        <v>24</v>
+      </c>
+      <c r="P42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -3921,10 +4584,16 @@
         <v>192</v>
       </c>
       <c r="K43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="L43" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>197</v>
       </c>
@@ -3958,8 +4627,26 @@
       <c r="K44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" t="s">
+        <v>9</v>
+      </c>
+      <c r="N44" t="s">
+        <v>9</v>
+      </c>
+      <c r="O44" t="s">
+        <v>24</v>
+      </c>
+      <c r="P44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>202</v>
       </c>
@@ -3993,8 +4680,26 @@
       <c r="K45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L45" t="s">
+        <v>9</v>
+      </c>
+      <c r="M45" t="s">
+        <v>9</v>
+      </c>
+      <c r="N45" t="s">
+        <v>9</v>
+      </c>
+      <c r="O45" t="s">
+        <v>24</v>
+      </c>
+      <c r="P45" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>207</v>
       </c>
@@ -4028,8 +4733,14 @@
       <c r="K46" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
+        <v>24</v>
+      </c>
+      <c r="M46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>209</v>
       </c>
@@ -4063,8 +4774,26 @@
       <c r="K47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" t="s">
+        <v>9</v>
+      </c>
+      <c r="N47" t="s">
+        <v>9</v>
+      </c>
+      <c r="O47" t="s">
+        <v>24</v>
+      </c>
+      <c r="P47" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>214</v>
       </c>
@@ -4098,8 +4827,26 @@
       <c r="K48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L48" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" t="s">
+        <v>9</v>
+      </c>
+      <c r="N48" t="s">
+        <v>9</v>
+      </c>
+      <c r="O48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P48" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4133,8 +4880,14 @@
       <c r="K49" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>24</v>
+      </c>
+      <c r="M49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>223</v>
       </c>
@@ -4168,8 +4921,26 @@
       <c r="K50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" t="s">
+        <v>9</v>
+      </c>
+      <c r="M50" t="s">
+        <v>9</v>
+      </c>
+      <c r="N50" t="s">
+        <v>9</v>
+      </c>
+      <c r="O50" t="s">
+        <v>24</v>
+      </c>
+      <c r="P50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>228</v>
       </c>
@@ -4203,8 +4974,26 @@
       <c r="K51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" t="s">
+        <v>9</v>
+      </c>
+      <c r="M51" t="s">
+        <v>9</v>
+      </c>
+      <c r="N51" t="s">
+        <v>9</v>
+      </c>
+      <c r="O51" t="s">
+        <v>24</v>
+      </c>
+      <c r="P51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>233</v>
       </c>
@@ -4238,8 +5027,26 @@
       <c r="K52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L52" t="s">
+        <v>9</v>
+      </c>
+      <c r="M52" t="s">
+        <v>9</v>
+      </c>
+      <c r="N52" t="s">
+        <v>9</v>
+      </c>
+      <c r="O52" t="s">
+        <v>9</v>
+      </c>
+      <c r="P52" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>237</v>
       </c>
@@ -4273,8 +5080,14 @@
       <c r="K53" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L53" t="s">
+        <v>24</v>
+      </c>
+      <c r="M53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>240</v>
       </c>
@@ -4296,8 +5109,14 @@
       <c r="K54" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
+        <v>24</v>
+      </c>
+      <c r="M54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>244</v>
       </c>
@@ -4331,8 +5150,14 @@
       <c r="K55" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55" t="s">
+        <v>24</v>
+      </c>
+      <c r="M55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>247</v>
       </c>
@@ -4366,8 +5191,26 @@
       <c r="K56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56" t="s">
+        <v>9</v>
+      </c>
+      <c r="M56" t="s">
+        <v>9</v>
+      </c>
+      <c r="N56" t="s">
+        <v>9</v>
+      </c>
+      <c r="O56" t="s">
+        <v>24</v>
+      </c>
+      <c r="P56" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>252</v>
       </c>
@@ -4401,8 +5244,26 @@
       <c r="K57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57" t="s">
+        <v>9</v>
+      </c>
+      <c r="M57" t="s">
+        <v>9</v>
+      </c>
+      <c r="N57" t="s">
+        <v>9</v>
+      </c>
+      <c r="O57" t="s">
+        <v>24</v>
+      </c>
+      <c r="P57" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>256</v>
       </c>
@@ -4436,8 +5297,26 @@
       <c r="K58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" t="s">
+        <v>9</v>
+      </c>
+      <c r="N58" t="s">
+        <v>9</v>
+      </c>
+      <c r="O58" t="s">
+        <v>9</v>
+      </c>
+      <c r="P58" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>260</v>
       </c>
@@ -4471,8 +5350,26 @@
       <c r="K59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L59" t="s">
+        <v>9</v>
+      </c>
+      <c r="M59" t="s">
+        <v>9</v>
+      </c>
+      <c r="N59" t="s">
+        <v>9</v>
+      </c>
+      <c r="O59" t="s">
+        <v>24</v>
+      </c>
+      <c r="P59" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>265</v>
       </c>
@@ -4494,8 +5391,14 @@
       <c r="K60" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L60" t="s">
+        <v>24</v>
+      </c>
+      <c r="M60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>269</v>
       </c>
@@ -4517,8 +5420,14 @@
       <c r="K61" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L61" t="s">
+        <v>24</v>
+      </c>
+      <c r="M61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>272</v>
       </c>
@@ -4540,8 +5449,26 @@
       <c r="K62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L62" t="s">
+        <v>9</v>
+      </c>
+      <c r="M62" t="s">
+        <v>9</v>
+      </c>
+      <c r="N62" t="s">
+        <v>9</v>
+      </c>
+      <c r="O62" t="s">
+        <v>24</v>
+      </c>
+      <c r="P62" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>277</v>
       </c>
@@ -4563,65 +5490,34 @@
       <c r="K63" t="s">
         <v>9</v>
       </c>
+      <c r="L63" t="s">
+        <v>9</v>
+      </c>
+      <c r="M63" t="s">
+        <v>9</v>
+      </c>
+      <c r="N63" t="s">
+        <v>9</v>
+      </c>
+      <c r="O63" t="s">
+        <v>24</v>
+      </c>
+      <c r="P63" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L63" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="afrikaans-afribooms"/>
-        <filter val="arabic-padt"/>
-        <filter val="armenian-armtdp"/>
-        <filter val="basque-bdt"/>
-        <filter val="bulgarian-btb"/>
-        <filter val="catalan-ancora"/>
-        <filter val="croatian-set"/>
-        <filter val="czech-cac"/>
-        <filter val="danish-ddt"/>
-        <filter val="dutch-alpino"/>
-        <filter val="english-ewt"/>
-        <filter val="estonian-edt"/>
-        <filter val="finnish-ftb"/>
-        <filter val="french-gsd"/>
-        <filter val="galician-ctg"/>
-        <filter val="german-gsd"/>
-        <filter val="greek-gdt"/>
-        <filter val="hebrew-htb"/>
-        <filter val="hindi-hdtb"/>
-        <filter val="hungarian-szeged"/>
-        <filter val="indonesian-gsd"/>
-        <filter val="italian-isdt"/>
-        <filter val="korean-gsd"/>
-        <filter val="latvian-lvtb"/>
-        <filter val="lithuanian-alksnis"/>
-        <filter val="norwegian-bokmaal"/>
-        <filter val="persian-seraji"/>
-        <filter val="polish-lfg"/>
-        <filter val="portuguese-gsd"/>
-        <filter val="romanian-rrt"/>
-        <filter val="russian-gsd"/>
-        <filter val="serbian-set"/>
-        <filter val="slovak-snk"/>
-        <filter val="slovenian-ssj"/>
-        <filter val="spanish-gsd"/>
-        <filter val="swedish-lines"/>
-        <filter val="tamil-ttb"/>
-        <filter val="turkish-imst"/>
-        <filter val="ukrainian-iu"/>
-        <filter val="urdu-udtb"/>
-        <filter val="vietnamese-vtb"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L64">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K64">
     <sortCondition ref="A2:A64"/>
   </sortState>
   <conditionalFormatting sqref="B1:E1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:Q1">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
cleaning up with new nonwords
</commit_message>
<xml_diff>
--- a/03_Materials/stimuli_options.xlsx
+++ b/03_Materials/stimuli_options.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/GitHub/SPAML/SPAML-PSA/03_Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2 projects/SPAML/SPAML-PSA/03_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A874944F-8FAD-6849-9689-3FC317312FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2139678-49D3-C644-9A78-182613D5FCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="21600" windowHeight="38400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="udpipe_languages" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">udpipe_languages!$A$2:$Q$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">udpipe_languages!$A$1:$Q$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2449,10 +2449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2525,34 +2526,34 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>288</v>
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>372</v>
       </c>
       <c r="C2" t="s">
-        <v>289</v>
+        <v>373</v>
       </c>
       <c r="D2" t="s">
-        <v>290</v>
+        <v>374</v>
       </c>
       <c r="E2" t="s">
-        <v>291</v>
+        <v>375</v>
       </c>
       <c r="F2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
         <v>9</v>
@@ -2578,34 +2579,34 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>364</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>365</v>
       </c>
       <c r="D3" t="s">
-        <v>294</v>
+        <v>366</v>
       </c>
       <c r="E3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F3" s="1">
-        <v>94093</v>
+        <v>367</v>
+      </c>
+      <c r="F3">
+        <v>449</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
@@ -2631,34 +2632,34 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="C4" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="E4" t="s">
-        <v>299</v>
-      </c>
-      <c r="F4" s="1">
-        <v>107923</v>
+        <v>315</v>
+      </c>
+      <c r="F4">
+        <v>832</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
         <v>9</v>
@@ -2682,7 +2683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2807,34 +2808,34 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>312</v>
+        <v>416</v>
       </c>
       <c r="C8" t="s">
-        <v>313</v>
+        <v>417</v>
       </c>
       <c r="D8" t="s">
-        <v>314</v>
+        <v>418</v>
       </c>
       <c r="E8" t="s">
-        <v>315</v>
+        <v>419</v>
       </c>
       <c r="F8">
-        <v>832</v>
+        <v>493</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>161</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>162</v>
       </c>
       <c r="K8" t="s">
         <v>9</v>
@@ -2860,34 +2861,34 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="C9" t="s">
-        <v>317</v>
+        <v>349</v>
       </c>
       <c r="D9" t="s">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c r="E9" t="s">
-        <v>319</v>
-      </c>
-      <c r="F9" s="1">
-        <v>157119</v>
+        <v>351</v>
+      </c>
+      <c r="F9">
+        <v>929</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="K9" t="s">
         <v>9</v>
@@ -2913,34 +2914,34 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>252</v>
       </c>
       <c r="B10" t="s">
-        <v>320</v>
+        <v>496</v>
       </c>
       <c r="C10" t="s">
-        <v>321</v>
+        <v>497</v>
       </c>
       <c r="D10" t="s">
-        <v>322</v>
+        <v>498</v>
       </c>
       <c r="E10" t="s">
-        <v>323</v>
+        <v>499</v>
       </c>
       <c r="F10" s="1">
-        <v>32350</v>
+        <v>1607</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>253</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>254</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>255</v>
       </c>
       <c r="K10" t="s">
         <v>9</v>
@@ -2966,34 +2967,22 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>324</v>
-      </c>
-      <c r="C11" t="s">
-        <v>325</v>
-      </c>
-      <c r="D11" t="s">
-        <v>326</v>
-      </c>
-      <c r="E11" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="F11" s="1">
-        <v>46468</v>
+        <v>9891</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>278</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>279</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>280</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>276</v>
       </c>
       <c r="K11" t="s">
         <v>9</v>
@@ -3019,34 +3008,34 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>328</v>
+        <v>380</v>
       </c>
       <c r="C12" t="s">
-        <v>329</v>
+        <v>381</v>
       </c>
       <c r="D12" t="s">
-        <v>330</v>
+        <v>382</v>
       </c>
       <c r="E12" t="s">
-        <v>331</v>
+        <v>383</v>
       </c>
       <c r="F12" s="1">
-        <v>143441</v>
+        <v>130769</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="K12" t="s">
         <v>9</v>
@@ -3072,34 +3061,34 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
       <c r="C13" t="s">
-        <v>333</v>
+        <v>433</v>
       </c>
       <c r="D13" t="s">
-        <v>334</v>
+        <v>434</v>
       </c>
       <c r="E13" t="s">
-        <v>335</v>
+        <v>435</v>
       </c>
       <c r="F13" s="1">
-        <v>446612</v>
+        <v>125371</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>175</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="I13" t="s">
-        <v>61</v>
+        <v>177</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>178</v>
       </c>
       <c r="K13" t="s">
         <v>9</v>
@@ -3123,7 +3112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -3166,34 +3155,34 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="C15" t="s">
-        <v>341</v>
+        <v>397</v>
       </c>
       <c r="D15" t="s">
-        <v>342</v>
+        <v>398</v>
       </c>
       <c r="E15" t="s">
-        <v>343</v>
+        <v>399</v>
       </c>
       <c r="F15" s="1">
-        <v>234457</v>
+        <v>134728</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="K15" t="s">
         <v>9</v>
@@ -3219,34 +3208,34 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="C16" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="D16" t="s">
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="E16" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="F16" s="1">
-        <v>28837</v>
+        <v>127204</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="K16" t="s">
         <v>9</v>
@@ -3272,34 +3261,34 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="C17" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="D17" t="s">
-        <v>350</v>
+        <v>378</v>
       </c>
       <c r="E17" t="s">
-        <v>351</v>
-      </c>
-      <c r="F17">
-        <v>929</v>
+        <v>379</v>
+      </c>
+      <c r="F17" s="1">
+        <v>126449</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="J17" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="K17" t="s">
         <v>9</v>
@@ -3325,34 +3314,34 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="B18" t="s">
-        <v>352</v>
+        <v>444</v>
       </c>
       <c r="C18" t="s">
-        <v>353</v>
+        <v>445</v>
       </c>
       <c r="D18" t="s">
-        <v>354</v>
+        <v>446</v>
       </c>
       <c r="E18" t="s">
-        <v>355</v>
+        <v>447</v>
       </c>
       <c r="F18" s="1">
-        <v>12185</v>
+        <v>131050</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="I18" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="J18" t="s">
-        <v>85</v>
+        <v>192</v>
       </c>
       <c r="K18" t="s">
         <v>9</v>
@@ -3378,34 +3367,34 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>356</v>
+        <v>328</v>
       </c>
       <c r="C19" t="s">
-        <v>357</v>
+        <v>329</v>
       </c>
       <c r="D19" t="s">
-        <v>358</v>
+        <v>330</v>
       </c>
       <c r="E19" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
       <c r="F19" s="1">
-        <v>64439</v>
+        <v>143441</v>
       </c>
       <c r="G19" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="I19" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="J19" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="K19" t="s">
         <v>9</v>
@@ -3431,34 +3420,34 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C20" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D20" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E20" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="F20" s="1">
-        <v>127204</v>
+        <v>12185</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J20" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="K20" t="s">
         <v>9</v>
@@ -3484,34 +3473,34 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s">
-        <v>364</v>
+        <v>436</v>
       </c>
       <c r="C21" t="s">
-        <v>365</v>
+        <v>437</v>
       </c>
       <c r="D21" t="s">
-        <v>366</v>
+        <v>438</v>
       </c>
       <c r="E21" t="s">
-        <v>367</v>
-      </c>
-      <c r="F21">
-        <v>449</v>
+        <v>439</v>
+      </c>
+      <c r="F21" s="1">
+        <v>14225</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="H21" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>99</v>
+        <v>181</v>
       </c>
       <c r="J21" t="s">
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="K21" t="s">
         <v>9</v>
@@ -3537,34 +3526,34 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>368</v>
+        <v>316</v>
       </c>
       <c r="C22" t="s">
-        <v>369</v>
+        <v>317</v>
       </c>
       <c r="D22" t="s">
-        <v>370</v>
+        <v>318</v>
       </c>
       <c r="E22" t="s">
-        <v>371</v>
+        <v>319</v>
       </c>
       <c r="F22" s="1">
-        <v>98679</v>
+        <v>157119</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="I22" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="K22" t="s">
         <v>9</v>
@@ -3590,34 +3579,34 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="B23" t="s">
-        <v>372</v>
+        <v>460</v>
       </c>
       <c r="C23" t="s">
-        <v>373</v>
+        <v>461</v>
       </c>
       <c r="D23" t="s">
-        <v>374</v>
+        <v>462</v>
       </c>
       <c r="E23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F23">
-        <v>102</v>
+        <v>463</v>
+      </c>
+      <c r="F23" s="1">
+        <v>18064</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>210</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="I23" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
       <c r="J23" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="K23" t="s">
         <v>9</v>
@@ -3632,45 +3621,45 @@
         <v>9</v>
       </c>
       <c r="O23" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="P23" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="Q23" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>376</v>
+        <v>472</v>
       </c>
       <c r="C24" t="s">
-        <v>377</v>
+        <v>473</v>
       </c>
       <c r="D24" t="s">
-        <v>378</v>
+        <v>474</v>
       </c>
       <c r="E24" t="s">
-        <v>379</v>
+        <v>475</v>
       </c>
       <c r="F24" s="1">
-        <v>126449</v>
+        <v>179648</v>
       </c>
       <c r="G24" t="s">
-        <v>111</v>
+        <v>224</v>
       </c>
       <c r="H24" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="J24" t="s">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="K24" t="s">
         <v>9</v>
@@ -3696,34 +3685,34 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>380</v>
+        <v>492</v>
       </c>
       <c r="C25" t="s">
-        <v>381</v>
+        <v>493</v>
       </c>
       <c r="D25" t="s">
-        <v>382</v>
+        <v>494</v>
       </c>
       <c r="E25" t="s">
-        <v>383</v>
+        <v>495</v>
       </c>
       <c r="F25" s="1">
-        <v>130769</v>
+        <v>189095</v>
       </c>
       <c r="G25" t="s">
-        <v>116</v>
+        <v>248</v>
       </c>
       <c r="H25" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="I25" t="s">
-        <v>118</v>
+        <v>250</v>
       </c>
       <c r="J25" t="s">
-        <v>119</v>
+        <v>251</v>
       </c>
       <c r="K25" t="s">
         <v>9</v>
@@ -3749,34 +3738,34 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>197</v>
       </c>
       <c r="B26" t="s">
-        <v>384</v>
+        <v>448</v>
       </c>
       <c r="C26" t="s">
-        <v>385</v>
+        <v>449</v>
       </c>
       <c r="D26" t="s">
-        <v>386</v>
+        <v>450</v>
       </c>
       <c r="E26" t="s">
-        <v>387</v>
-      </c>
-      <c r="F26">
-        <v>9</v>
+        <v>451</v>
+      </c>
+      <c r="F26" s="1">
+        <v>205322</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
       <c r="I26" t="s">
-        <v>123</v>
+        <v>200</v>
       </c>
       <c r="J26" t="s">
-        <v>124</v>
+        <v>201</v>
       </c>
       <c r="K26" t="s">
         <v>9</v>
@@ -3791,45 +3780,45 @@
         <v>9</v>
       </c>
       <c r="O26" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="P26" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="Q26" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="C27" t="s">
-        <v>389</v>
+        <v>413</v>
       </c>
       <c r="D27" t="s">
-        <v>390</v>
+        <v>414</v>
       </c>
       <c r="E27" t="s">
-        <v>391</v>
+        <v>415</v>
       </c>
       <c r="F27" s="1">
-        <v>21628</v>
+        <v>1976</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="H27" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="I27" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="J27" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="K27" t="s">
         <v>9</v>
@@ -3853,7 +3842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -3896,34 +3885,34 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="C29" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="D29" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="E29" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="F29" s="1">
-        <v>134728</v>
+        <v>2193</v>
       </c>
       <c r="G29" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="H29" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="I29" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="J29" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="K29" t="s">
         <v>9</v>
@@ -3949,22 +3938,34 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>340</v>
+      </c>
+      <c r="C30" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E30" t="s">
+        <v>343</v>
       </c>
       <c r="F30" s="1">
-        <v>3546</v>
+        <v>234457</v>
       </c>
       <c r="G30" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="H30" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="I30" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="J30" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="K30" t="s">
         <v>9</v>
@@ -3988,7 +3989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -4029,7 +4030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -4072,34 +4073,34 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="C33" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="D33" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="E33" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="F33" s="1">
-        <v>2193</v>
+        <v>21628</v>
       </c>
       <c r="G33" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="H33" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="I33" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="J33" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="K33" t="s">
         <v>9</v>
@@ -4125,34 +4126,34 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>412</v>
+        <v>440</v>
       </c>
       <c r="C34" t="s">
-        <v>413</v>
+        <v>441</v>
       </c>
       <c r="D34" t="s">
-        <v>414</v>
+        <v>442</v>
       </c>
       <c r="E34" t="s">
-        <v>415</v>
+        <v>443</v>
       </c>
       <c r="F34" s="1">
-        <v>1976</v>
+        <v>278833</v>
       </c>
       <c r="G34" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="I34" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="J34" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="K34" t="s">
         <v>9</v>
@@ -4178,34 +4179,34 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>416</v>
+        <v>344</v>
       </c>
       <c r="C35" t="s">
-        <v>417</v>
+        <v>345</v>
       </c>
       <c r="D35" t="s">
-        <v>418</v>
+        <v>346</v>
       </c>
       <c r="E35" t="s">
-        <v>419</v>
-      </c>
-      <c r="F35">
-        <v>493</v>
+        <v>347</v>
+      </c>
+      <c r="F35" s="1">
+        <v>28837</v>
       </c>
       <c r="G35" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="H35" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="I35" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="J35" t="s">
-        <v>162</v>
+        <v>75</v>
       </c>
       <c r="K35" t="s">
         <v>9</v>
@@ -4229,7 +4230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -4270,7 +4271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>167</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>171</v>
       </c>
@@ -4354,34 +4355,22 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" t="s">
-        <v>432</v>
-      </c>
-      <c r="C39" t="s">
-        <v>433</v>
-      </c>
-      <c r="D39" t="s">
-        <v>434</v>
-      </c>
-      <c r="E39" t="s">
-        <v>435</v>
+        <v>139</v>
       </c>
       <c r="F39" s="1">
-        <v>125371</v>
+        <v>3546</v>
       </c>
       <c r="G39" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="H39" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="I39" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="J39" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="K39" t="s">
         <v>9</v>
@@ -4407,34 +4396,34 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>436</v>
+        <v>320</v>
       </c>
       <c r="C40" t="s">
-        <v>437</v>
+        <v>321</v>
       </c>
       <c r="D40" t="s">
-        <v>438</v>
+        <v>322</v>
       </c>
       <c r="E40" t="s">
-        <v>439</v>
+        <v>323</v>
       </c>
       <c r="F40" s="1">
-        <v>14225</v>
+        <v>32350</v>
       </c>
       <c r="G40" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="H40" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="I40" t="s">
-        <v>181</v>
+        <v>46</v>
       </c>
       <c r="J40" t="s">
-        <v>182</v>
+        <v>47</v>
       </c>
       <c r="K40" t="s">
         <v>9</v>
@@ -4460,34 +4449,22 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" t="s">
-        <v>440</v>
-      </c>
-      <c r="C41" t="s">
-        <v>441</v>
-      </c>
-      <c r="D41" t="s">
-        <v>442</v>
-      </c>
-      <c r="E41" t="s">
-        <v>443</v>
+        <v>272</v>
       </c>
       <c r="F41" s="1">
-        <v>278833</v>
+        <v>29074</v>
       </c>
       <c r="G41" t="s">
-        <v>184</v>
+        <v>273</v>
       </c>
       <c r="H41" t="s">
-        <v>185</v>
+        <v>274</v>
       </c>
       <c r="I41" t="s">
-        <v>186</v>
+        <v>275</v>
       </c>
       <c r="J41" t="s">
-        <v>187</v>
+        <v>276</v>
       </c>
       <c r="K41" t="s">
         <v>9</v>
@@ -4513,34 +4490,34 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="B42" t="s">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c r="C42" t="s">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c r="D42" t="s">
-        <v>446</v>
+        <v>478</v>
       </c>
       <c r="E42" t="s">
-        <v>447</v>
+        <v>479</v>
       </c>
       <c r="F42" s="1">
-        <v>131050</v>
+        <v>41084</v>
       </c>
       <c r="G42" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="H42" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="I42" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="J42" t="s">
-        <v>192</v>
+        <v>232</v>
       </c>
       <c r="K42" t="s">
         <v>9</v>
@@ -4564,7 +4541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -4595,34 +4572,34 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>197</v>
+        <v>120</v>
       </c>
       <c r="B44" t="s">
-        <v>448</v>
+        <v>384</v>
       </c>
       <c r="C44" t="s">
-        <v>449</v>
+        <v>385</v>
       </c>
       <c r="D44" t="s">
-        <v>450</v>
+        <v>386</v>
       </c>
       <c r="E44" t="s">
-        <v>451</v>
-      </c>
-      <c r="F44" s="1">
-        <v>205322</v>
+        <v>387</v>
+      </c>
+      <c r="F44">
+        <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>198</v>
+        <v>121</v>
       </c>
       <c r="H44" t="s">
-        <v>199</v>
+        <v>122</v>
       </c>
       <c r="I44" t="s">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="J44" t="s">
-        <v>201</v>
+        <v>124</v>
       </c>
       <c r="K44" t="s">
         <v>9</v>
@@ -4637,45 +4614,45 @@
         <v>9</v>
       </c>
       <c r="O44" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="P44" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="Q44" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="B45" t="s">
-        <v>452</v>
+        <v>480</v>
       </c>
       <c r="C45" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="D45" t="s">
-        <v>454</v>
+        <v>482</v>
       </c>
       <c r="E45" t="s">
-        <v>455</v>
-      </c>
-      <c r="F45" s="1">
-        <v>55976</v>
+        <v>483</v>
+      </c>
+      <c r="F45">
+        <v>32</v>
       </c>
       <c r="G45" t="s">
-        <v>203</v>
+        <v>26</v>
       </c>
       <c r="H45" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="I45" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="J45" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="K45" t="s">
         <v>9</v>
@@ -4690,16 +4667,16 @@
         <v>9</v>
       </c>
       <c r="O45" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="P45" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="Q45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>207</v>
       </c>
@@ -4742,34 +4719,34 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>209</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>460</v>
+        <v>324</v>
       </c>
       <c r="C47" t="s">
-        <v>461</v>
+        <v>325</v>
       </c>
       <c r="D47" t="s">
-        <v>462</v>
+        <v>326</v>
       </c>
       <c r="E47" t="s">
-        <v>463</v>
+        <v>327</v>
       </c>
       <c r="F47" s="1">
-        <v>18064</v>
+        <v>46468</v>
       </c>
       <c r="G47" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
       <c r="H47" t="s">
-        <v>211</v>
+        <v>50</v>
       </c>
       <c r="I47" t="s">
-        <v>212</v>
+        <v>51</v>
       </c>
       <c r="J47" t="s">
-        <v>213</v>
+        <v>52</v>
       </c>
       <c r="K47" t="s">
         <v>9</v>
@@ -4795,34 +4772,34 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B48" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="C48" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="D48" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="E48" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="F48" s="1">
-        <v>60405</v>
+        <v>55976</v>
       </c>
       <c r="G48" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="H48" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="I48" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="J48" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="K48" t="s">
         <v>9</v>
@@ -4846,7 +4823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4889,34 +4866,34 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>223</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>472</v>
+        <v>332</v>
       </c>
       <c r="C50" t="s">
-        <v>473</v>
+        <v>333</v>
       </c>
       <c r="D50" t="s">
-        <v>474</v>
+        <v>334</v>
       </c>
       <c r="E50" t="s">
-        <v>475</v>
+        <v>335</v>
       </c>
       <c r="F50" s="1">
-        <v>179648</v>
+        <v>446612</v>
       </c>
       <c r="G50" t="s">
-        <v>224</v>
+        <v>59</v>
       </c>
       <c r="H50" t="s">
-        <v>225</v>
+        <v>60</v>
       </c>
       <c r="I50" t="s">
-        <v>226</v>
+        <v>61</v>
       </c>
       <c r="J50" t="s">
-        <v>227</v>
+        <v>62</v>
       </c>
       <c r="K50" t="s">
         <v>9</v>
@@ -4942,34 +4919,34 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="B51" t="s">
-        <v>476</v>
+        <v>500</v>
       </c>
       <c r="C51" t="s">
-        <v>477</v>
+        <v>501</v>
       </c>
       <c r="D51" t="s">
-        <v>478</v>
+        <v>502</v>
       </c>
       <c r="E51" t="s">
-        <v>479</v>
-      </c>
-      <c r="F51" s="1">
-        <v>41084</v>
+        <v>503</v>
+      </c>
+      <c r="F51">
+        <v>35</v>
       </c>
       <c r="G51" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="H51" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="I51" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="J51" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
       <c r="K51" t="s">
         <v>9</v>
@@ -4984,45 +4961,45 @@
         <v>9</v>
       </c>
       <c r="O51" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="P51" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="Q51" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s">
-        <v>480</v>
+        <v>504</v>
       </c>
       <c r="C52" t="s">
-        <v>481</v>
+        <v>505</v>
       </c>
       <c r="D52" t="s">
-        <v>482</v>
+        <v>506</v>
       </c>
       <c r="E52" t="s">
-        <v>483</v>
-      </c>
-      <c r="F52">
-        <v>32</v>
+        <v>507</v>
+      </c>
+      <c r="F52" s="1">
+        <v>5165</v>
       </c>
       <c r="G52" t="s">
-        <v>26</v>
+        <v>261</v>
       </c>
       <c r="H52" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="I52" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="J52" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="K52" t="s">
         <v>9</v>
@@ -5037,16 +5014,16 @@
         <v>9</v>
       </c>
       <c r="O52" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="P52" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="Q52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>237</v>
       </c>
@@ -5087,7 +5064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>240</v>
       </c>
@@ -5116,7 +5093,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>244</v>
       </c>
@@ -5159,34 +5136,34 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>247</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>492</v>
+        <v>356</v>
       </c>
       <c r="C56" t="s">
-        <v>493</v>
+        <v>357</v>
       </c>
       <c r="D56" t="s">
-        <v>494</v>
+        <v>358</v>
       </c>
       <c r="E56" t="s">
-        <v>495</v>
+        <v>359</v>
       </c>
       <c r="F56" s="1">
-        <v>189095</v>
+        <v>64439</v>
       </c>
       <c r="G56" t="s">
-        <v>248</v>
+        <v>87</v>
       </c>
       <c r="H56" t="s">
-        <v>249</v>
+        <v>88</v>
       </c>
       <c r="I56" t="s">
-        <v>250</v>
+        <v>89</v>
       </c>
       <c r="J56" t="s">
-        <v>251</v>
+        <v>90</v>
       </c>
       <c r="K56" t="s">
         <v>9</v>
@@ -5212,34 +5189,34 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B57" t="s">
-        <v>496</v>
+        <v>464</v>
       </c>
       <c r="C57" t="s">
-        <v>497</v>
+        <v>465</v>
       </c>
       <c r="D57" t="s">
-        <v>498</v>
+        <v>466</v>
       </c>
       <c r="E57" t="s">
-        <v>499</v>
+        <v>467</v>
       </c>
       <c r="F57" s="1">
-        <v>1607</v>
+        <v>60405</v>
       </c>
       <c r="G57" t="s">
-        <v>165</v>
+        <v>215</v>
       </c>
       <c r="H57" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="I57" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
       <c r="J57" t="s">
-        <v>255</v>
+        <v>218</v>
       </c>
       <c r="K57" t="s">
         <v>9</v>
@@ -5265,34 +5242,34 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>256</v>
-      </c>
-      <c r="B58" t="s">
-        <v>500</v>
+        <v>4</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>501</v>
+        <v>289</v>
       </c>
       <c r="D58" t="s">
-        <v>502</v>
+        <v>290</v>
       </c>
       <c r="E58" t="s">
-        <v>503</v>
+        <v>291</v>
       </c>
       <c r="F58">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" t="s">
-        <v>257</v>
+        <v>6</v>
       </c>
       <c r="I58" t="s">
-        <v>258</v>
+        <v>7</v>
       </c>
       <c r="J58" t="s">
-        <v>259</v>
+        <v>8</v>
       </c>
       <c r="K58" t="s">
         <v>9</v>
@@ -5318,34 +5295,34 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>260</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>504</v>
+        <v>292</v>
       </c>
       <c r="C59" t="s">
-        <v>505</v>
+        <v>293</v>
       </c>
       <c r="D59" t="s">
-        <v>506</v>
+        <v>294</v>
       </c>
       <c r="E59" t="s">
-        <v>507</v>
+        <v>295</v>
       </c>
       <c r="F59" s="1">
-        <v>5165</v>
+        <v>94093</v>
       </c>
       <c r="G59" t="s">
-        <v>261</v>
+        <v>11</v>
       </c>
       <c r="H59" t="s">
-        <v>262</v>
+        <v>12</v>
       </c>
       <c r="I59" t="s">
-        <v>263</v>
+        <v>13</v>
       </c>
       <c r="J59" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="K59" t="s">
         <v>9</v>
@@ -5369,7 +5346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>265</v>
       </c>
@@ -5398,7 +5375,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>269</v>
       </c>
@@ -5429,22 +5406,34 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>272</v>
+        <v>101</v>
+      </c>
+      <c r="B62" t="s">
+        <v>368</v>
+      </c>
+      <c r="C62" t="s">
+        <v>369</v>
+      </c>
+      <c r="D62" t="s">
+        <v>370</v>
+      </c>
+      <c r="E62" t="s">
+        <v>371</v>
       </c>
       <c r="F62" s="1">
-        <v>29074</v>
+        <v>98679</v>
       </c>
       <c r="G62" t="s">
-        <v>273</v>
+        <v>102</v>
       </c>
       <c r="H62" t="s">
-        <v>274</v>
+        <v>103</v>
       </c>
       <c r="I62" t="s">
-        <v>275</v>
+        <v>104</v>
       </c>
       <c r="J62" t="s">
-        <v>276</v>
+        <v>105</v>
       </c>
       <c r="K62" t="s">
         <v>9</v>
@@ -5470,22 +5459,34 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>277</v>
+        <v>15</v>
+      </c>
+      <c r="B63" t="s">
+        <v>296</v>
+      </c>
+      <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" t="s">
+        <v>298</v>
+      </c>
+      <c r="E63" t="s">
+        <v>299</v>
       </c>
       <c r="F63" s="1">
-        <v>9891</v>
+        <v>107923</v>
       </c>
       <c r="G63" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
       <c r="H63" t="s">
-        <v>279</v>
+        <v>17</v>
       </c>
       <c r="I63" t="s">
-        <v>280</v>
+        <v>18</v>
       </c>
       <c r="J63" t="s">
-        <v>276</v>
+        <v>19</v>
       </c>
       <c r="K63" t="s">
         <v>9</v>
@@ -5510,6 +5511,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q63" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q63">
+      <sortCondition ref="H1:H63"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K64">
     <sortCondition ref="A2:A64"/>
   </sortState>
@@ -5520,8 +5531,9 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B58" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>